<commit_message>
Softstart on recorded RMS voltages + minmimum init times in sheet
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MKT\Desktop\MTB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B5696B-84D0-435A-8319-25C9F1CF708B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5088E7-EA50-46D3-A5DB-4D515B9ED851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="38700" windowHeight="15435" tabRatio="298" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="225" windowWidth="28800" windowHeight="15435" tabRatio="298" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="479">
   <si>
     <t>Range</t>
   </si>
@@ -1542,6 +1542,12 @@
   </si>
   <si>
     <t>Solbakken_EMT</t>
+  </si>
+  <si>
+    <t>Atleast 1s</t>
+  </si>
+  <si>
+    <t>Atleast 0,1s</t>
   </si>
 </sst>
 </file>
@@ -2139,7 +2145,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -2553,6 +2559,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20 % - Farve3" xfId="1" builtinId="38"/>
@@ -2843,7 +2852,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3140,12 +3149,14 @@
         <v>28</v>
       </c>
       <c r="B21" s="45">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="C21" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="31"/>
+      <c r="E21" s="163" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
@@ -3157,7 +3168,9 @@
       <c r="C22" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="31"/>
+      <c r="E22" s="163" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
@@ -3228,6 +3241,16 @@
   <mergeCells count="1">
     <mergeCell ref="G14:I14"/>
   </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B21" xr:uid="{47C97EA5-00CA-4E06-B63F-2ED7D203FE97}">
+      <formula1>1</formula1>
+      <formula2>99999999</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22" xr:uid="{B8F7F6F9-D94A-485B-BBB8-9B81074994B0}">
+      <formula1>0.1</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -31628,6 +31651,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
@@ -31636,15 +31668,6 @@
     <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -31897,6 +31920,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2288FB7-E85A-4FE8-9E7A-FE572FF16064}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="888ccf44-0d39-41a2-ab17-f7efb2bf6977"/>
@@ -31909,14 +31940,6 @@
     <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>